<commit_message>
개발팀 Additional Merge 2
</commit_message>
<xml_diff>
--- a/Assets/Dialogs/DialogDB_Lake.xlsx
+++ b/Assets/Dialogs/DialogDB_Lake.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\LGHNH_Project\Assets\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB62A71-A70D-41D3-9767-973C8733CCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E41BC11-5BA0-49F2-88B8-6CDC85ADCFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{CDE8FF25-D89C-42B6-B5F0-688FBD2DA1BA}"/>
   </bookViews>
@@ -825,7 +825,7 @@
   <dimension ref="A1:H1068"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="15" customHeight="1"/>

</xml_diff>